<commit_message>
02-12-2022 Comparator case study
</commit_message>
<xml_diff>
--- a/Updates.xlsx
+++ b/Updates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Java Full Stack\JAVA\CORE\KTG\shankar\9-10 pm oct 2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F48DAF89-82B7-4771-961B-4EC7B74063CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C73E784-EB83-49BE-B8CA-4FFCCFCA2287}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="53">
   <si>
     <t>Concepts</t>
   </si>
@@ -133,9 +133,6 @@
     <t>case study</t>
   </si>
   <si>
-    <t>jpa+hibernate</t>
-  </si>
-  <si>
     <t>spring+springboot</t>
   </si>
   <si>
@@ -169,9 +166,6 @@
     <t>1:20 minutes</t>
   </si>
   <si>
-    <t>java 8 features ,collection</t>
-  </si>
-  <si>
     <t>life cycle,thread class methods,synchronization,thread communication</t>
   </si>
   <si>
@@ -179,6 +173,18 @@
   </si>
   <si>
     <t>complete multi threading</t>
+  </si>
+  <si>
+    <t>collection,list,set and few methods</t>
+  </si>
+  <si>
+    <t xml:space="preserve">list and set methods map </t>
+  </si>
+  <si>
+    <t>1:20mintues</t>
+  </si>
+  <si>
+    <t>case study,comparable ,comparator</t>
   </si>
 </sst>
 </file>
@@ -614,7 +620,7 @@
   <dimension ref="A3:M165"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -852,10 +858,10 @@
         <v>32</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I17" s="4"/>
     </row>
@@ -864,13 +870,13 @@
         <v>44887</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G18" s="6" t="s">
         <v>8</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I18" s="4"/>
     </row>
@@ -880,13 +886,13 @@
         <v>44888</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G19" s="6" t="s">
         <v>8</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I19" s="4"/>
     </row>
@@ -895,10 +901,10 @@
         <v>44889</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H20" s="4" t="s">
         <v>28</v>
@@ -910,10 +916,10 @@
         <v>44893</v>
       </c>
       <c r="F21" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="G21" s="6" t="s">
         <v>45</v>
-      </c>
-      <c r="G21" s="6" t="s">
-        <v>46</v>
       </c>
       <c r="H21" s="4" t="s">
         <v>28</v>
@@ -925,24 +931,28 @@
         <v>44894</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G22" s="4" t="s">
         <v>8</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I22" s="11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="E23" s="7">
+        <v>44895</v>
+      </c>
+      <c r="F23" s="4" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="E23" s="4"/>
-      <c r="F23" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="G23" s="4"/>
+      <c r="G23" s="4" t="s">
+        <v>8</v>
+      </c>
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
       <c r="M23" s="10" t="s">
@@ -950,27 +960,35 @@
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="E24" s="4"/>
+      <c r="E24" s="7">
+        <v>44896</v>
+      </c>
       <c r="F24" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="G24" s="4"/>
+        <v>50</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>51</v>
+      </c>
       <c r="H24" s="4"/>
       <c r="I24" s="4"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="E25" s="4"/>
+      <c r="E25" s="7">
+        <v>44897</v>
+      </c>
       <c r="F25" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="G25" s="4"/>
+        <v>52</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>8</v>
+      </c>
       <c r="H25" s="4"/>
       <c r="I25" s="4"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="E26" s="4"/>
       <c r="F26" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
@@ -988,7 +1006,7 @@
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="E28" s="4"/>
       <c r="F28" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>

</xml_diff>